<commit_message>
merged bike tracks with same name
and recalculated for each city
</commit_message>
<xml_diff>
--- a/datapreparation/citystatus.xlsx
+++ b/datapreparation/citystatus.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="31280" yWindow="-9660" windowWidth="28800" windowHeight="16420" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16420" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="35">
   <si>
     <t>berlin</t>
   </si>
@@ -131,7 +131,7 @@
     <t>rome</t>
   </si>
   <si>
-    <t>X C bike</t>
+    <t>sao paolo</t>
   </si>
 </sst>
 </file>
@@ -513,10 +513,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:S17"/>
+  <dimension ref="A1:S18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -729,7 +729,7 @@
         <v>24</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="K6" s="7" t="s">
         <v>24</v>
@@ -1059,6 +1059,11 @@
       <c r="Q17" s="12"/>
       <c r="R17" s="12"/>
     </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A18" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="C1:E1"/>

</xml_diff>

<commit_message>
added city meta data
</commit_message>
<xml_diff>
--- a/datapreparation/citystatus.xlsx
+++ b/datapreparation/citystatus.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16420" tabRatio="500"/>
+    <workbookView xWindow="47200" yWindow="-8820" windowWidth="28800" windowHeight="16420" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="35">
   <si>
     <t>berlin</t>
   </si>
@@ -516,7 +516,7 @@
   <dimension ref="A1:S18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+      <selection activeCell="T10" sqref="T10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -622,10 +622,16 @@
         <v>24</v>
       </c>
       <c r="M3" s="4"/>
-      <c r="N3" s="3"/>
-      <c r="P3" s="3"/>
+      <c r="N3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>24</v>
+      </c>
       <c r="Q3" s="3"/>
-      <c r="R3" s="3"/>
+      <c r="R3" s="3" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -660,10 +666,16 @@
         <v>24</v>
       </c>
       <c r="M4" s="6"/>
-      <c r="N4" s="5"/>
-      <c r="P4" s="5"/>
+      <c r="N4" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="P4" s="5" t="s">
+        <v>24</v>
+      </c>
       <c r="Q4" s="5"/>
-      <c r="R4" s="5"/>
+      <c r="R4" s="5" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
@@ -699,10 +711,16 @@
         <v>24</v>
       </c>
       <c r="M5" s="4"/>
-      <c r="N5" s="3"/>
-      <c r="P5" s="3"/>
+      <c r="N5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="P5" s="3" t="s">
+        <v>24</v>
+      </c>
       <c r="Q5" s="3"/>
-      <c r="R5" s="3"/>
+      <c r="R5" s="3" t="s">
+        <v>24</v>
+      </c>
       <c r="S5" s="9"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.2">
@@ -738,11 +756,15 @@
         <v>24</v>
       </c>
       <c r="M6" s="8"/>
-      <c r="N6" s="7"/>
+      <c r="N6" s="7" t="s">
+        <v>24</v>
+      </c>
       <c r="O6" s="9"/>
       <c r="P6" s="7"/>
       <c r="Q6" s="7"/>
-      <c r="R6" s="7"/>
+      <c r="R6" s="7" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
@@ -778,10 +800,14 @@
         <v>24</v>
       </c>
       <c r="M7" s="4"/>
-      <c r="N7" s="3"/>
+      <c r="N7" s="3" t="s">
+        <v>24</v>
+      </c>
       <c r="P7" s="3"/>
       <c r="Q7" s="3"/>
-      <c r="R7" s="3"/>
+      <c r="R7" s="3" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
@@ -816,10 +842,14 @@
         <v>24</v>
       </c>
       <c r="M8" s="6"/>
-      <c r="N8" s="5"/>
+      <c r="N8" s="5" t="s">
+        <v>24</v>
+      </c>
       <c r="P8" s="5"/>
       <c r="Q8" s="5"/>
-      <c r="R8" s="5"/>
+      <c r="R8" s="5" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
@@ -855,10 +885,14 @@
         <v>24</v>
       </c>
       <c r="M9" s="4"/>
-      <c r="N9" s="3"/>
+      <c r="N9" s="3" t="s">
+        <v>24</v>
+      </c>
       <c r="P9" s="3"/>
       <c r="Q9" s="3"/>
-      <c r="R9" s="3"/>
+      <c r="R9" s="3" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
@@ -893,10 +927,14 @@
         <v>24</v>
       </c>
       <c r="M10" s="6"/>
-      <c r="N10" s="5"/>
+      <c r="N10" s="5" t="s">
+        <v>24</v>
+      </c>
       <c r="P10" s="5"/>
       <c r="Q10" s="5"/>
-      <c r="R10" s="5"/>
+      <c r="R10" s="5" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
@@ -952,10 +990,14 @@
         <v>24</v>
       </c>
       <c r="M12" s="6"/>
-      <c r="N12" s="5"/>
+      <c r="N12" s="5" t="s">
+        <v>24</v>
+      </c>
       <c r="P12" s="5"/>
       <c r="Q12" s="5"/>
-      <c r="R12" s="5"/>
+      <c r="R12" s="5" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">

</xml_diff>